<commit_message>
se agrego material a la lista
</commit_message>
<xml_diff>
--- a/materiales.xlsx
+++ b/materiales.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Desktop\estacion_climatica\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>elemento</t>
   </si>
@@ -45,9 +45,6 @@
   </si>
   <si>
     <t>1 Fotorresistencia (ldr)</t>
-  </si>
-  <si>
-    <t>Arduino uno</t>
   </si>
   <si>
     <t>10 jumpers macho-macho</t>
@@ -115,11 +112,11 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -405,7 +402,7 @@
   <dimension ref="D2:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,10 +412,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="1"/>
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2"/>
     </row>
     <row r="3" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
@@ -455,37 +452,32 @@
     </row>
     <row r="9" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D10" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D16" s="1" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="4:5" x14ac:dyDescent="0.25">
-      <c r="D16" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>